<commit_message>
combined 8 virginia scenarios
</commit_message>
<xml_diff>
--- a/projects/virginia/data/data_virginia.xlsx
+++ b/projects/virginia/data/data_virginia.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB41A6E4-E412-C04A-895D-09828957A55C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1A4CB3-ADE4-B549-9FA0-7CE58784C3FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="941" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-44960" yWindow="2660" windowWidth="33600" windowHeight="20540" tabRatio="941" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>

</xml_diff>

<commit_message>
NG/Storage/Solar CF Update, 15% RM, and Validation
</commit_message>
<xml_diff>
--- a/projects/virginia/data/data_virginia.xlsx
+++ b/projects/virginia/data/data_virginia.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CE2BDD-0860-0C4B-ABEC-8C2E207C6C40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4DF397-AC3A-8443-928D-6B204222B0D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="460" windowWidth="51200" windowHeight="21140" tabRatio="941" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51200" yWindow="460" windowWidth="51200" windowHeight="21140" tabRatio="941" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2501" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2521" uniqueCount="259">
   <si>
     <t>connection</t>
   </si>
@@ -812,6 +812,9 @@
   </si>
   <si>
     <t>Ref_MinCapacity</t>
+  </si>
+  <si>
+    <t>EX_NG_GT</t>
   </si>
 </sst>
 </file>
@@ -1935,10 +1938,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2248,10 +2251,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>112</v>
+        <v>258</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>92</v>
+        <v>187</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>102</v>
@@ -2266,7 +2269,7 @@
         <v>126</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>126</v>
@@ -2274,10 +2277,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>200</v>
+        <v>112</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>199</v>
+        <v>92</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>102</v>
@@ -2292,7 +2295,7 @@
         <v>126</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>126</v>
@@ -2300,10 +2303,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>113</v>
+        <v>200</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>93</v>
+        <v>199</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>102</v>
@@ -2318,7 +2321,7 @@
         <v>126</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>126</v>
@@ -2326,10 +2329,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>216</v>
+        <v>113</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>102</v>
@@ -2338,27 +2341,24 @@
         <v>127</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>126</v>
       </c>
       <c r="G15" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="J15">
-        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>102</v>
@@ -2367,24 +2367,27 @@
         <v>127</v>
       </c>
       <c r="E16" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="F16" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>126</v>
+      <c r="J16">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>230</v>
+        <v>120</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>102</v>
@@ -2407,10 +2410,10 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>102</v>
+        <v>230</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>102</v>
@@ -2419,97 +2422,97 @@
         <v>127</v>
       </c>
       <c r="E18" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F18" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="G18" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="H18" s="5" t="s">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="J18">
+      <c r="E19" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="J19">
         <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="J19">
-        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="C20" s="16" t="s">
         <v>102</v>
       </c>
       <c r="D20" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="E20" s="16" t="s">
         <v>126</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>127</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>127</v>
       </c>
       <c r="G20" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="H20" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="H20" s="16" t="s">
-        <v>126</v>
+      <c r="J20">
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
-        <v>189</v>
+        <v>115</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>185</v>
+        <v>120</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="E21" s="5" t="s">
+      <c r="D21" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="E21" s="16" t="s">
         <v>127</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>127</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H21" s="16" t="s">
         <v>126</v>
@@ -2517,10 +2520,10 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>102</v>
@@ -2543,10 +2546,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>102</v>
@@ -2569,18 +2572,18 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
-        <v>116</v>
+        <v>192</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="5" t="s">
         <v>127</v>
       </c>
       <c r="F24" s="16" t="s">
@@ -2595,7 +2598,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>187</v>
@@ -2604,7 +2607,7 @@
         <v>102</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E25" s="16" t="s">
         <v>127</v>
@@ -2621,10 +2624,10 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>92</v>
+        <v>187</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>102</v>
@@ -2639,7 +2642,7 @@
         <v>127</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H26" s="16" t="s">
         <v>126</v>
@@ -2647,10 +2650,10 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>102</v>
@@ -2672,72 +2675,72 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D28" s="5" t="s">
+      <c r="A28" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="E28" s="16" t="s">
         <v>127</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>126</v>
       </c>
       <c r="F28" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="G28" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="H28" s="16" t="s">
         <v>126</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="J28">
-        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>99</v>
       </c>
       <c r="D29" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>127</v>
       </c>
       <c r="F29" s="16" t="s">
         <v>127</v>
       </c>
       <c r="G29" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H29" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H29" s="5" t="s">
-        <v>126</v>
+      <c r="J29">
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>174</v>
+        <v>129</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>187</v>
+        <v>120</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>99</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>127</v>
@@ -2746,7 +2749,7 @@
         <v>127</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>126</v>
@@ -2754,7 +2757,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>130</v>
+        <v>174</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>187</v>
@@ -2763,7 +2766,7 @@
         <v>99</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>127</v>
@@ -2780,10 +2783,10 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>92</v>
+        <v>187</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>99</v>
@@ -2798,7 +2801,7 @@
         <v>127</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>126</v>
@@ -2806,13 +2809,13 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>252</v>
+        <v>131</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>126</v>
@@ -2830,23 +2833,49 @@
         <v>126</v>
       </c>
     </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D24:E33 D20:E20 G20:H20 G24:H33 F20:F33 D3:H15 D19:H19">
+  <conditionalFormatting sqref="D25:E34 D21:E21 G21:H21 G25:H34 F21:F34 D20:H20 D3:H16">
     <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21:E23 G21:H23">
+  <conditionalFormatting sqref="D22:E24 G22:H24">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16:H17">
+  <conditionalFormatting sqref="D17:H18">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18:H18">
+  <conditionalFormatting sqref="D19:H19">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2858,10 +2887,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2938,10 +2967,10 @@
         <v>103</v>
       </c>
       <c r="B3" s="8">
-        <v>30</v>
+        <v>29.1</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="D3" s="8">
         <v>39.4</v>
@@ -2966,7 +2995,7 @@
         <v>76</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="D4" s="8">
         <v>29.9</v>
@@ -2991,7 +3020,7 @@
         <v>80</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="D5" s="8">
         <v>40</v>
@@ -3016,7 +3045,7 @@
         <v>85</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="D6" s="8">
         <v>35.299999999999997</v>
@@ -3041,7 +3070,7 @@
         <v>85</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="D7" s="8">
         <v>34.6</v>
@@ -3066,7 +3095,7 @@
         <v>85</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="D8" s="8">
         <v>34.1</v>
@@ -3088,10 +3117,10 @@
         <v>109</v>
       </c>
       <c r="B9" s="8">
-        <v>21</v>
+        <v>23.3</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="D9" s="8">
         <v>90</v>
@@ -3116,7 +3145,7 @@
         <v>56</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="D10" s="5">
         <v>19</v>
@@ -3138,10 +3167,10 @@
         <v>111</v>
       </c>
       <c r="B11" s="8">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="D11" s="8">
         <v>54.1</v>
@@ -3160,18 +3189,18 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
-        <v>112</v>
+        <v>258</v>
       </c>
       <c r="B12" s="5">
-        <v>23.2</v>
+        <v>30</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="D12" s="5">
-        <v>20</v>
-      </c>
-      <c r="E12" s="8" t="s">
+        <v>54.1</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>197</v>
       </c>
       <c r="F12" s="8"/>
@@ -3185,16 +3214,16 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
-        <v>200</v>
+        <v>112</v>
       </c>
       <c r="B13" s="5">
-        <v>93.6</v>
+        <v>23.2</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="D13" s="5">
-        <v>32.6</v>
+        <v>20</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>197</v>
@@ -3202,7 +3231,7 @@
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="5">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>197</v>
@@ -3210,24 +3239,24 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B14" s="5">
-        <v>61.9</v>
+        <v>93.6</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="D14" s="5">
-        <v>35.299999999999997</v>
+        <v>32.6</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="8"/>
       <c r="G14" s="8"/>
-      <c r="H14" s="8">
-        <v>45</v>
+      <c r="H14" s="5">
+        <v>100</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>197</v>
@@ -3235,24 +3264,24 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="B15" s="5">
-        <v>14.8</v>
+        <v>61.9</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="D15" s="5">
-        <v>80</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>197</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="8"/>
-      <c r="H15" s="5">
-        <v>100</v>
+      <c r="H15" s="8">
+        <v>45</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>197</v>
@@ -3260,24 +3289,24 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
-        <v>113</v>
+        <v>216</v>
       </c>
       <c r="B16" s="5">
-        <v>48.5</v>
+        <v>50</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="D16" s="5">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="8"/>
       <c r="H16" s="5">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>197</v>
@@ -3285,24 +3314,24 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
-        <v>231</v>
+        <v>113</v>
       </c>
       <c r="B17" s="5">
-        <v>61</v>
-      </c>
-      <c r="C17" s="5" t="s">
+        <v>48.5</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="D17" s="24">
-        <v>35.299999999999997</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="F17" s="5"/>
+      <c r="D17" s="5">
+        <v>50</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>197</v>
@@ -3310,24 +3339,24 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="B18" s="16">
-        <v>16.7</v>
+        <v>231</v>
+      </c>
+      <c r="B18" s="5">
+        <v>61</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="D18" s="16">
-        <v>85</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16">
-        <v>15</v>
+        <v>218</v>
+      </c>
+      <c r="D18" s="24">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="5">
+        <v>50</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>197</v>
@@ -3335,16 +3364,16 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
-        <v>217</v>
+        <v>114</v>
       </c>
       <c r="B19" s="16">
-        <v>14.8</v>
+        <v>50</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>197</v>
       </c>
       <c r="D19" s="16">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>197</v>
@@ -3352,7 +3381,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
       <c r="H19" s="16">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>197</v>
@@ -3360,24 +3389,24 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>115</v>
+        <v>217</v>
       </c>
       <c r="B20" s="16">
-        <v>61.9</v>
+        <v>50</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>197</v>
       </c>
       <c r="D20" s="16">
-        <v>35.299999999999997</v>
+        <v>80</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>197</v>
       </c>
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
-      <c r="H20" s="17">
-        <v>45</v>
+      <c r="H20" s="16">
+        <v>100</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>197</v>
@@ -3385,24 +3414,24 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
-        <v>189</v>
+        <v>115</v>
       </c>
       <c r="B21" s="16">
-        <v>30</v>
+        <v>61.9</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="D21" s="19">
-        <v>39.4</v>
+      <c r="D21" s="16">
+        <v>35.299999999999997</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>197</v>
       </c>
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
-      <c r="H21" s="16">
-        <v>40</v>
+      <c r="H21" s="17">
+        <v>45</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>197</v>
@@ -3410,16 +3439,16 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B22" s="16">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>197</v>
       </c>
       <c r="D22" s="19">
-        <v>51.7</v>
+        <v>39.4</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>197</v>
@@ -3427,7 +3456,7 @@
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
       <c r="H22" s="16">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>197</v>
@@ -3435,7 +3464,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B23" s="16">
         <v>87</v>
@@ -3452,7 +3481,7 @@
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
       <c r="H23" s="16">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>197</v>
@@ -3460,16 +3489,16 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="B24" s="18">
-        <v>55</v>
+        <v>192</v>
+      </c>
+      <c r="B24" s="16">
+        <v>87</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="D24" s="16">
-        <v>54.1</v>
+      <c r="D24" s="19">
+        <v>51.7</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>197</v>
@@ -3477,7 +3506,7 @@
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
       <c r="H24" s="16">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>197</v>
@@ -3485,24 +3514,24 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="B25" s="16">
-        <v>30</v>
+        <v>116</v>
+      </c>
+      <c r="B25" s="18">
+        <v>87</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>197</v>
       </c>
       <c r="D25" s="16">
-        <v>42.47</v>
+        <v>54.1</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>197</v>
       </c>
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
-      <c r="H25" s="17">
-        <v>55</v>
+      <c r="H25" s="16">
+        <v>30</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>197</v>
@@ -3510,24 +3539,24 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B26" s="16">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>197</v>
       </c>
       <c r="D26" s="16">
-        <v>20</v>
+        <v>42.47</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>197</v>
       </c>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
-      <c r="H26" s="16">
-        <v>30</v>
+      <c r="H26" s="17">
+        <v>55</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>197</v>
@@ -3535,16 +3564,16 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B27" s="16">
-        <v>48.5</v>
+        <v>23.2</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>197</v>
       </c>
       <c r="D27" s="16">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>197</v>
@@ -3560,24 +3589,24 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="B28" s="5">
-        <v>16.7</v>
+        <v>119</v>
+      </c>
+      <c r="B28" s="16">
+        <v>48.5</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="D28" s="8">
-        <v>85</v>
+      <c r="D28" s="16">
+        <v>50</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8">
-        <v>15</v>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16">
+        <v>30</v>
       </c>
       <c r="I28" s="5" t="s">
         <v>197</v>
@@ -3585,24 +3614,24 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B29" s="5">
-        <v>61.9</v>
+        <v>50</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="D29" s="5">
-        <v>35.299999999999997</v>
+      <c r="D29" s="8">
+        <v>85</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="F29" s="5"/>
+      <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>197</v>
@@ -3610,24 +3639,24 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="B30" s="9">
-        <v>55</v>
+        <v>129</v>
+      </c>
+      <c r="B30" s="5">
+        <v>61.9</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="D30" s="8">
-        <v>54.1</v>
+      <c r="D30" s="5">
+        <v>35.299999999999997</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>197</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="8"/>
-      <c r="H30" s="5">
-        <v>30</v>
+      <c r="H30" s="8">
+        <v>45</v>
       </c>
       <c r="I30" s="5" t="s">
         <v>197</v>
@@ -3635,10 +3664,10 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="B31" s="5">
-        <v>55</v>
+        <v>174</v>
+      </c>
+      <c r="B31" s="9">
+        <v>87</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>197</v>
@@ -3651,8 +3680,8 @@
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="8"/>
-      <c r="H31" s="8">
-        <v>55</v>
+      <c r="H31" s="5">
+        <v>30</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>197</v>
@@ -3660,16 +3689,16 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B32" s="5">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="D32" s="5">
-        <v>20</v>
+      <c r="D32" s="8">
+        <v>54.1</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>197</v>
@@ -3677,7 +3706,7 @@
       <c r="F32" s="5"/>
       <c r="G32" s="8"/>
       <c r="H32" s="8">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>197</v>
@@ -3685,16 +3714,16 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="23" t="s">
-        <v>252</v>
+        <v>131</v>
       </c>
       <c r="B33" s="5">
-        <v>46</v>
+        <v>23.2</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>197</v>
       </c>
       <c r="D33" s="5">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>197</v>
@@ -3705,6 +3734,31 @@
         <v>30</v>
       </c>
       <c r="I33" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="B34" s="5">
+        <v>46</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="D34" s="5">
+        <v>50</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="F34" s="5"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8">
+        <v>30</v>
+      </c>
+      <c r="I34" s="5" t="s">
         <v>197</v>
       </c>
     </row>
@@ -3716,10 +3770,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4032,35 +4086,31 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
-        <v>112</v>
+        <v>258</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="E12" s="5">
-        <v>19</v>
-      </c>
-      <c r="F12" s="5">
-        <v>-2.67</v>
-      </c>
+      <c r="E12" s="9">
+        <v>13</v>
+      </c>
+      <c r="F12" s="9"/>
       <c r="G12" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="H12" s="8">
-        <v>0</v>
-      </c>
-      <c r="I12" s="5">
-        <v>0</v>
-      </c>
+      <c r="H12" s="5">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="I12" s="8"/>
       <c r="J12" s="10" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
-        <v>200</v>
+        <v>112</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -4068,218 +4118,220 @@
         <v>197</v>
       </c>
       <c r="E13" s="5">
-        <v>119</v>
-      </c>
-      <c r="F13" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="F13" s="5">
+        <v>-2.67</v>
+      </c>
       <c r="G13" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="H13" s="5">
-        <v>0.55600000000000005</v>
-      </c>
-      <c r="I13" s="5"/>
+      <c r="H13" s="8">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0</v>
+      </c>
       <c r="J13" s="10" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
-        <v>207</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
+        <v>200</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="E14" s="6">
-        <v>123</v>
-      </c>
-      <c r="F14" s="6"/>
+      <c r="E14" s="5">
+        <v>119</v>
+      </c>
+      <c r="F14" s="5"/>
       <c r="G14" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="H14" s="21">
-        <v>1.39</v>
-      </c>
-      <c r="I14" s="21"/>
+      <c r="H14" s="5">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="I14" s="5"/>
       <c r="J14" s="10" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="5" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="E15" s="6">
-        <v>3</v>
+        <v>123</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="10" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="H15" s="21">
-        <v>2.78</v>
+        <v>1.39</v>
       </c>
       <c r="I15" s="21"/>
       <c r="J15" s="10" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
+        <v>216</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
       <c r="D16" s="5" t="s">
-        <v>197</v>
+        <v>229</v>
       </c>
       <c r="E16" s="6">
-        <v>108</v>
-      </c>
-      <c r="F16" s="6">
-        <v>-2.65</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F16" s="6"/>
       <c r="G16" s="10" t="s">
-        <v>197</v>
+        <v>229</v>
       </c>
       <c r="H16" s="21">
-        <v>0</v>
-      </c>
-      <c r="I16" s="21">
-        <v>0</v>
-      </c>
+        <v>2.78</v>
+      </c>
+      <c r="I16" s="21"/>
       <c r="J16" s="10" t="s">
-        <v>197</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
-        <v>231</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
+        <v>113</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
         <v>197</v>
       </c>
       <c r="E17" s="6">
-        <v>123</v>
-      </c>
-      <c r="F17" s="6"/>
+        <v>108</v>
+      </c>
+      <c r="F17" s="6">
+        <v>-2.65</v>
+      </c>
       <c r="G17" s="10" t="s">
         <v>197</v>
       </c>
       <c r="H17" s="21">
-        <v>1.39</v>
-      </c>
-      <c r="I17" s="21"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="21">
+        <v>0</v>
+      </c>
       <c r="J17" s="10" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="B18" s="17">
-        <v>1544</v>
-      </c>
-      <c r="C18" s="17"/>
+        <v>231</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
       <c r="D18" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="E18" s="17">
-        <v>38.6</v>
-      </c>
-      <c r="F18" s="17"/>
+      <c r="E18" s="6">
+        <v>123</v>
+      </c>
+      <c r="F18" s="6"/>
       <c r="G18" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="H18" s="17">
-        <v>0</v>
-      </c>
-      <c r="I18" s="17"/>
+      <c r="H18" s="21">
+        <v>1.39</v>
+      </c>
+      <c r="I18" s="21"/>
       <c r="J18" s="10" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
-        <v>217</v>
+        <v>114</v>
       </c>
       <c r="B19" s="17">
-        <v>4300</v>
+        <v>1544</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="5" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="E19" s="17">
-        <v>3</v>
+        <v>38.6</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="10" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="H19" s="17">
-        <v>2.78</v>
+        <v>0</v>
       </c>
       <c r="I19" s="17"/>
       <c r="J19" s="10" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>115</v>
+        <v>217</v>
       </c>
       <c r="B20" s="17">
-        <v>4348</v>
+        <v>4300</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="5" t="s">
-        <v>197</v>
+        <v>229</v>
       </c>
       <c r="E20" s="17">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="10" t="s">
-        <v>197</v>
+        <v>229</v>
       </c>
       <c r="H20" s="17">
-        <v>1.39</v>
+        <v>2.78</v>
       </c>
       <c r="I20" s="17"/>
       <c r="J20" s="10" t="s">
-        <v>197</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
-        <v>189</v>
+        <v>115</v>
       </c>
       <c r="B21" s="17">
-        <v>3603</v>
+        <v>4348</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="5" t="s">
         <v>197</v>
       </c>
       <c r="E21" s="17">
-        <v>40</v>
+        <v>123</v>
       </c>
       <c r="F21" s="17"/>
       <c r="G21" s="10" t="s">
         <v>197</v>
       </c>
       <c r="H21" s="17">
-        <v>1.1100000000000001</v>
+        <v>1.39</v>
       </c>
       <c r="I21" s="17"/>
       <c r="J21" s="10" t="s">
@@ -4288,24 +4340,24 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B22" s="17">
-        <v>1044</v>
+        <v>3603</v>
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="5" t="s">
         <v>197</v>
       </c>
       <c r="E22" s="17">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="F22" s="17"/>
       <c r="G22" s="10" t="s">
         <v>197</v>
       </c>
       <c r="H22" s="17">
-        <v>0.55600000000000005</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="I22" s="17"/>
       <c r="J22" s="10" t="s">
@@ -4314,7 +4366,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B23" s="17">
         <v>1044</v>
@@ -4340,19 +4392,19 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="B24" s="20">
+        <v>192</v>
+      </c>
+      <c r="B24" s="17">
         <v>1044</v>
       </c>
-      <c r="C24" s="20"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="E24" s="22">
+      <c r="E24" s="17">
         <v>13</v>
       </c>
-      <c r="F24" s="22"/>
+      <c r="F24" s="17"/>
       <c r="G24" s="10" t="s">
         <v>197</v>
       </c>
@@ -4366,24 +4418,24 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="B25" s="17">
-        <v>943</v>
-      </c>
-      <c r="C25" s="17"/>
+        <v>116</v>
+      </c>
+      <c r="B25" s="20">
+        <v>1044</v>
+      </c>
+      <c r="C25" s="20"/>
       <c r="D25" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="E25" s="17">
-        <v>11</v>
-      </c>
-      <c r="F25" s="17"/>
+      <c r="E25" s="22">
+        <v>13</v>
+      </c>
+      <c r="F25" s="22"/>
       <c r="G25" s="10" t="s">
         <v>197</v>
       </c>
       <c r="H25" s="17">
-        <v>1.1100000000000001</v>
+        <v>0.55600000000000005</v>
       </c>
       <c r="I25" s="17"/>
       <c r="J25" s="10" t="s">
@@ -4392,60 +4444,48 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B26" s="17">
-        <v>1600</v>
-      </c>
-      <c r="C26" s="17">
-        <v>-2.6</v>
-      </c>
+        <v>943</v>
+      </c>
+      <c r="C26" s="17"/>
       <c r="D26" s="5" t="s">
         <v>197</v>
       </c>
       <c r="E26" s="17">
-        <v>19</v>
-      </c>
-      <c r="F26" s="5">
-        <v>-2.67</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F26" s="17"/>
       <c r="G26" s="10" t="s">
         <v>197</v>
       </c>
       <c r="H26" s="17">
-        <v>0</v>
-      </c>
-      <c r="I26" s="17">
-        <v>0</v>
-      </c>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="I26" s="17"/>
       <c r="J26" s="10" t="s">
         <v>197</v>
-      </c>
-      <c r="K26">
-        <v>0.08</v>
-      </c>
-      <c r="L26" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B27" s="17">
-        <v>4443</v>
+        <v>1600</v>
       </c>
       <c r="C27" s="17">
-        <v>-2.75</v>
+        <v>-2.6</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>197</v>
       </c>
       <c r="E27" s="17">
-        <v>130</v>
-      </c>
-      <c r="F27" s="17">
-        <v>-2.65</v>
+        <v>19</v>
+      </c>
+      <c r="F27" s="5">
+        <v>-2.67</v>
       </c>
       <c r="G27" s="10" t="s">
         <v>197</v>
@@ -4468,76 +4508,88 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="B28" s="6">
-        <v>1544</v>
-      </c>
-      <c r="C28" s="6"/>
+        <v>119</v>
+      </c>
+      <c r="B28" s="17">
+        <v>4443</v>
+      </c>
+      <c r="C28" s="17">
+        <v>-2.75</v>
+      </c>
       <c r="D28" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="E28" s="6">
-        <v>38.6</v>
-      </c>
-      <c r="F28" s="6"/>
+      <c r="E28" s="17">
+        <v>130</v>
+      </c>
+      <c r="F28" s="17">
+        <v>-2.65</v>
+      </c>
       <c r="G28" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="H28" s="21">
-        <v>0</v>
-      </c>
-      <c r="I28" s="21"/>
+      <c r="H28" s="17">
+        <v>0</v>
+      </c>
+      <c r="I28" s="17">
+        <v>0</v>
+      </c>
       <c r="J28" s="10" t="s">
         <v>197</v>
+      </c>
+      <c r="K28">
+        <v>0.08</v>
+      </c>
+      <c r="L28" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="B29" s="17">
-        <v>4348</v>
-      </c>
-      <c r="C29" s="17"/>
+        <v>128</v>
+      </c>
+      <c r="B29" s="6">
+        <v>1544</v>
+      </c>
+      <c r="C29" s="6"/>
       <c r="D29" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="E29" s="17">
-        <v>123</v>
-      </c>
-      <c r="F29" s="17"/>
+      <c r="E29" s="6">
+        <v>38.6</v>
+      </c>
+      <c r="F29" s="6"/>
       <c r="G29" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="H29" s="17">
-        <v>1.39</v>
-      </c>
-      <c r="I29" s="17"/>
+      <c r="H29" s="21">
+        <v>0</v>
+      </c>
+      <c r="I29" s="21"/>
       <c r="J29" s="10" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="B30" s="20">
-        <v>1044</v>
-      </c>
-      <c r="C30" s="20"/>
+        <v>129</v>
+      </c>
+      <c r="B30" s="17">
+        <v>4348</v>
+      </c>
+      <c r="C30" s="17"/>
       <c r="D30" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="E30" s="22">
-        <v>13</v>
-      </c>
-      <c r="F30" s="22"/>
+      <c r="E30" s="17">
+        <v>123</v>
+      </c>
+      <c r="F30" s="17"/>
       <c r="G30" s="10" t="s">
         <v>197</v>
       </c>
       <c r="H30" s="17">
-        <v>0.55600000000000005</v>
+        <v>1.39</v>
       </c>
       <c r="I30" s="17"/>
       <c r="J30" s="10" t="s">
@@ -4546,24 +4598,24 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="B31" s="17">
-        <v>943</v>
-      </c>
-      <c r="C31" s="17"/>
+        <v>174</v>
+      </c>
+      <c r="B31" s="20">
+        <v>1044</v>
+      </c>
+      <c r="C31" s="20"/>
       <c r="D31" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="E31" s="17">
-        <v>11</v>
-      </c>
-      <c r="F31" s="17"/>
+      <c r="E31" s="22">
+        <v>13</v>
+      </c>
+      <c r="F31" s="22"/>
       <c r="G31" s="10" t="s">
         <v>197</v>
       </c>
       <c r="H31" s="17">
-        <v>1.1100000000000001</v>
+        <v>0.55600000000000005</v>
       </c>
       <c r="I31" s="17"/>
       <c r="J31" s="10" t="s">
@@ -4572,60 +4624,48 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="B32" s="6">
-        <v>2052</v>
-      </c>
-      <c r="C32" s="6">
-        <v>-2.96</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="B32" s="17">
+        <v>943</v>
+      </c>
+      <c r="C32" s="17"/>
       <c r="D32" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="E32" s="6">
-        <v>18</v>
-      </c>
-      <c r="F32" s="6">
-        <v>-3.37</v>
-      </c>
+      <c r="E32" s="17">
+        <v>11</v>
+      </c>
+      <c r="F32" s="17"/>
       <c r="G32" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="H32" s="6">
-        <v>0</v>
-      </c>
-      <c r="I32" s="6">
-        <v>0</v>
-      </c>
+      <c r="H32" s="17">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="I32" s="17"/>
       <c r="J32" s="10" t="s">
         <v>197</v>
-      </c>
-      <c r="K32">
-        <v>0.08</v>
-      </c>
-      <c r="L32" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="23" t="s">
-        <v>252</v>
+        <v>131</v>
       </c>
       <c r="B33" s="6">
-        <v>6598</v>
+        <v>2052</v>
       </c>
       <c r="C33" s="6">
-        <v>-4.12</v>
+        <v>-2.96</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>197</v>
       </c>
       <c r="E33" s="6">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="F33" s="6">
-        <v>-2.67</v>
+        <v>-3.37</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>197</v>
@@ -4647,11 +4687,49 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
+      <c r="A34" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="B34" s="6">
+        <v>6598</v>
+      </c>
+      <c r="C34" s="6">
+        <v>-4.12</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E34" s="6">
+        <v>108</v>
+      </c>
+      <c r="F34" s="6">
+        <v>-2.67</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H34" s="6">
+        <v>0</v>
+      </c>
+      <c r="I34" s="6">
+        <v>0</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="K34">
+        <v>0.08</v>
+      </c>
+      <c r="L34" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4661,10 +4739,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4754,7 +4832,9 @@
       <c r="C3" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H3" s="33"/>
+      <c r="H3" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
@@ -4766,7 +4846,9 @@
       <c r="C4" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H4" s="33"/>
+      <c r="H4" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -4778,7 +4860,9 @@
       <c r="C5" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H5" s="33"/>
+      <c r="H5" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -4790,7 +4874,9 @@
       <c r="C6" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H6" s="33"/>
+      <c r="H6" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
@@ -4802,7 +4888,9 @@
       <c r="C7" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H7" s="33"/>
+      <c r="H7" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
@@ -4814,7 +4902,9 @@
       <c r="C8" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H8" s="33"/>
+      <c r="H8" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
@@ -4822,7 +4912,9 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
-      <c r="H9" s="33"/>
+      <c r="H9" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
@@ -4830,7 +4922,9 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
-      <c r="H10" s="33"/>
+      <c r="H10" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
@@ -4840,51 +4934,59 @@
         <v>1</v>
       </c>
       <c r="C11" s="5"/>
-      <c r="H11" s="33"/>
+      <c r="H11" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B12" s="5"/>
+        <v>258</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
       <c r="C12" s="5"/>
-      <c r="H12" s="33"/>
+      <c r="H12" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="B13" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="H13" s="33"/>
+        <v>112</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="H13" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="H14" s="33"/>
+        <v>200</v>
+      </c>
+      <c r="B14" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="H14" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="H15" s="33">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
         <v>113</v>
-      </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="33"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
-        <v>114</v>
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -4892,11 +4994,13 @@
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
-      <c r="H16" s="33"/>
+      <c r="H16" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
-        <v>217</v>
+        <v>114</v>
       </c>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -4904,46 +5008,44 @@
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
-      <c r="H17" s="33"/>
+      <c r="H17" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="B18" s="19">
-        <v>0.01</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>132</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
-      <c r="H18" s="33"/>
+      <c r="H18" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="B19" s="19">
-        <v>0.93</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>132</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
-      <c r="H19" s="33"/>
+      <c r="H19" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
-        <v>190</v>
+        <v>115</v>
       </c>
       <c r="B20" s="19">
-        <v>0.93</v>
+        <v>0.01</v>
       </c>
       <c r="C20" s="19" t="s">
         <v>132</v>
@@ -4952,119 +5054,179 @@
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
-      <c r="H20" s="33"/>
+      <c r="H20" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="B21" s="16">
-        <v>1</v>
-      </c>
-      <c r="C21" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="B21" s="19">
+        <v>0.93</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>132</v>
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
-      <c r="H21" s="33"/>
+      <c r="H21" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
+        <v>190</v>
+      </c>
+      <c r="B22" s="19">
+        <v>0.93</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>132</v>
+      </c>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
-      <c r="H22" s="33"/>
+      <c r="H22" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
+        <v>192</v>
+      </c>
+      <c r="B23" s="16">
+        <v>1</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>132</v>
+      </c>
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
-      <c r="H23" s="33"/>
+      <c r="H23" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
-      <c r="D24" s="19">
-        <v>20000</v>
-      </c>
+      <c r="D24" s="19"/>
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
-      <c r="H24" s="33"/>
+      <c r="H24" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="33">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19">
+        <v>20000</v>
+      </c>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="33">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="D25">
+      <c r="D27">
         <v>5200</v>
       </c>
-      <c r="H25" s="33"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="H26" s="33"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B27" s="5">
-        <v>1</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="H27" s="33"/>
+      <c r="H27" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="H28" s="33"/>
+        <v>128</v>
+      </c>
+      <c r="H28" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="H29" s="33"/>
+        <v>129</v>
+      </c>
+      <c r="B29" s="5">
+        <v>1</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H29" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D30">
-        <v>20000</v>
-      </c>
-      <c r="F30" s="2"/>
-      <c r="H30" s="33"/>
+        <v>174</v>
+      </c>
+      <c r="H30" s="33">
+        <v>2020</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="H31" s="33">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D32">
+        <v>20000</v>
+      </c>
+      <c r="F32" s="2"/>
+      <c r="H32" s="33">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D31">
+      <c r="D33">
         <v>10000</v>
       </c>
-      <c r="H31" s="33"/>
+      <c r="H33" s="33">
+        <v>2020</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5074,10 +5236,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5223,7 +5385,7 @@
         <v>111</v>
       </c>
       <c r="B11">
-        <v>8596</v>
+        <v>5769</v>
       </c>
       <c r="C11">
         <v>1995</v>
@@ -5248,85 +5410,99 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>112</v>
+        <v>258</v>
       </c>
       <c r="B13">
-        <v>392.5</v>
+        <v>4245</v>
       </c>
       <c r="C13">
-        <v>2015</v>
+        <v>1995</v>
       </c>
       <c r="D13" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>392.5</v>
       </c>
       <c r="C14">
         <v>2015</v>
       </c>
       <c r="D14" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>200</v>
+        <v>113</v>
       </c>
       <c r="B15">
-        <v>3568</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>2015</v>
       </c>
       <c r="D15" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B16">
-        <v>1475</v>
+        <v>3568</v>
       </c>
       <c r="C16">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="D16" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="B17">
-        <v>3241</v>
+        <v>1475</v>
       </c>
       <c r="C17">
-        <v>1970</v>
+        <v>2013</v>
       </c>
       <c r="D17" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>216</v>
+      </c>
+      <c r="B18">
+        <v>3241</v>
+      </c>
+      <c r="C18">
+        <v>1970</v>
+      </c>
+      <c r="D18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>231</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>578</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>2015</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>218</v>
       </c>
     </row>
@@ -5585,7 +5761,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5613,7 +5789,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
   </sheetData>
@@ -5625,8 +5801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E290"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5784,7 +5960,7 @@
         <v>171</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>6.5151613927753579E-2</v>
       </c>
       <c r="E9" t="s">
         <v>145</v>
@@ -5801,7 +5977,7 @@
         <v>172</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>0.51710729986794368</v>
       </c>
       <c r="E10" t="s">
         <v>145</v>
@@ -5818,7 +5994,7 @@
         <v>173</v>
       </c>
       <c r="D11">
-        <v>0.77007469706240006</v>
+        <v>1.4080047807699383</v>
       </c>
       <c r="E11" t="s">
         <v>145</v>
@@ -5835,7 +6011,7 @@
         <v>48</v>
       </c>
       <c r="D12">
-        <v>1.281333465104</v>
+        <v>2.3170650920214642</v>
       </c>
       <c r="E12" t="s">
         <v>145</v>
@@ -5852,7 +6028,7 @@
         <v>49</v>
       </c>
       <c r="D13">
-        <v>2.3646544747520002</v>
+        <v>2.9657135215552537</v>
       </c>
       <c r="E13" t="s">
         <v>145</v>
@@ -5869,7 +6045,7 @@
         <v>50</v>
       </c>
       <c r="D14">
-        <v>3.0280632685280002</v>
+        <v>3.3662870467880248</v>
       </c>
       <c r="E14" t="s">
         <v>145</v>
@@ -5886,7 +6062,7 @@
         <v>51</v>
       </c>
       <c r="D15">
-        <v>3.0209459722159995</v>
+        <v>3.5088012971599545</v>
       </c>
       <c r="E15" t="s">
         <v>145</v>
@@ -5903,7 +6079,7 @@
         <v>52</v>
       </c>
       <c r="D16">
-        <v>2.795326114032</v>
+        <v>3.4843814252043517</v>
       </c>
       <c r="E16" t="s">
         <v>145</v>
@@ -5920,7 +6096,7 @@
         <v>53</v>
       </c>
       <c r="D17">
-        <v>2.2633913706480002</v>
+        <v>3.3241196529762793</v>
       </c>
       <c r="E17" t="s">
         <v>145</v>
@@ -5937,7 +6113,7 @@
         <v>54</v>
       </c>
       <c r="D18">
-        <v>1.8486804048160002</v>
+        <v>2.9143805058255179</v>
       </c>
       <c r="E18" t="s">
         <v>145</v>
@@ -5954,7 +6130,7 @@
         <v>55</v>
       </c>
       <c r="D19">
-        <v>1.2956684382880002</v>
+        <v>2.2592273038797788</v>
       </c>
       <c r="E19" t="s">
         <v>145</v>
@@ -5971,7 +6147,7 @@
         <v>56</v>
       </c>
       <c r="D20">
-        <v>0.53186179455679994</v>
+        <v>1.4246780502482324</v>
       </c>
       <c r="E20" t="s">
         <v>145</v>
@@ -5988,7 +6164,7 @@
         <v>57</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>0.52272896711966943</v>
       </c>
       <c r="E21" t="s">
         <v>145</v>
@@ -6005,7 +6181,7 @@
         <v>58</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>5.9752854253380804E-2</v>
       </c>
       <c r="E22" t="s">
         <v>145</v>
@@ -6192,7 +6368,7 @@
         <v>171</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>0.17960986159169545</v>
       </c>
       <c r="E33" t="s">
         <v>145</v>
@@ -6209,7 +6385,7 @@
         <v>172</v>
       </c>
       <c r="D34">
-        <v>6.8030477198099994E-3</v>
+        <v>0.96234111880046114</v>
       </c>
       <c r="E34" t="s">
         <v>145</v>
@@ -6226,7 +6402,7 @@
         <v>173</v>
       </c>
       <c r="D35">
-        <v>0.62784163046800001</v>
+        <v>2.0715934256055348</v>
       </c>
       <c r="E35" t="s">
         <v>145</v>
@@ -6243,7 +6419,7 @@
         <v>48</v>
       </c>
       <c r="D36">
-        <v>1.5458351067</v>
+        <v>3.0472691272587453</v>
       </c>
       <c r="E36" t="s">
         <v>145</v>
@@ -6260,7 +6436,7 @@
         <v>49</v>
       </c>
       <c r="D37">
-        <v>2.4637406089799998</v>
+        <v>3.7972426951172618</v>
       </c>
       <c r="E37" t="s">
         <v>145</v>
@@ -6277,7 +6453,7 @@
         <v>50</v>
       </c>
       <c r="D38">
-        <v>3.00512030807</v>
+        <v>4.2245385428681281</v>
       </c>
       <c r="E38" t="s">
         <v>145</v>
@@ -6294,7 +6470,7 @@
         <v>51</v>
       </c>
       <c r="D39">
-        <v>3.5308931214800006</v>
+        <v>4.3589632833525549</v>
       </c>
       <c r="E39" t="s">
         <v>145</v>
@@ -6311,7 +6487,7 @@
         <v>52</v>
       </c>
       <c r="D40">
-        <v>3.69605507635</v>
+        <v>4.2665792003075742</v>
       </c>
       <c r="E40" t="s">
         <v>145</v>
@@ -6328,7 +6504,7 @@
         <v>53</v>
       </c>
       <c r="D41">
-        <v>3.3774587455400007</v>
+        <v>4.1128616878123783</v>
       </c>
       <c r="E41" t="s">
         <v>145</v>
@@ -6345,7 +6521,7 @@
         <v>54</v>
       </c>
       <c r="D42">
-        <v>2.7769065497900001</v>
+        <v>3.7373002691272581</v>
       </c>
       <c r="E42" t="s">
         <v>145</v>
@@ -6362,7 +6538,7 @@
         <v>55</v>
       </c>
       <c r="D43">
-        <v>1.9586883649700004</v>
+        <v>3.016870049980775</v>
       </c>
       <c r="E43" t="s">
         <v>145</v>
@@ -6379,7 +6555,7 @@
         <v>56</v>
       </c>
       <c r="D44">
-        <v>1.0106574399199999</v>
+        <v>2.1133196847366391</v>
       </c>
       <c r="E44" t="s">
         <v>145</v>
@@ -6396,7 +6572,7 @@
         <v>57</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>1.0572132833525567</v>
       </c>
       <c r="E45" t="s">
         <v>145</v>
@@ -6413,7 +6589,7 @@
         <v>58</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>0.24639331026528258</v>
       </c>
       <c r="E46" t="s">
         <v>145</v>
@@ -6430,7 +6606,7 @@
         <v>59</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>4.8337178008458275E-3</v>
       </c>
       <c r="E47" t="s">
         <v>145</v>
@@ -6583,7 +6759,7 @@
         <v>170</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>1.1826555003928239E-3</v>
       </c>
       <c r="E56" t="s">
         <v>145</v>
@@ -6600,7 +6776,7 @@
         <v>171</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>0.1545210872072614</v>
       </c>
       <c r="E57" t="s">
         <v>145</v>
@@ -6617,7 +6793,7 @@
         <v>172</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>0.88859744579843858</v>
       </c>
       <c r="E58" t="s">
         <v>145</v>
@@ -6634,7 +6810,7 @@
         <v>173</v>
       </c>
       <c r="D59">
-        <v>0.77007469706240006</v>
+        <v>1.8354981361683627</v>
       </c>
       <c r="E59" t="s">
         <v>145</v>
@@ -6651,7 +6827,7 @@
         <v>48</v>
       </c>
       <c r="D60">
-        <v>1.281333465104</v>
+        <v>2.5212421643849341</v>
       </c>
       <c r="E60" t="s">
         <v>145</v>
@@ -6668,7 +6844,7 @@
         <v>49</v>
       </c>
       <c r="D61">
-        <v>2.3646544747520002</v>
+        <v>2.8966652458084687</v>
       </c>
       <c r="E61" t="s">
         <v>145</v>
@@ -6685,7 +6861,7 @@
         <v>50</v>
       </c>
       <c r="D62">
-        <v>3.0280632685280002</v>
+        <v>3.0148905103388319</v>
       </c>
       <c r="E62" t="s">
         <v>145</v>
@@ -6702,7 +6878,7 @@
         <v>51</v>
       </c>
       <c r="D63">
-        <v>3.0209459722159995</v>
+        <v>2.9434981528843425</v>
       </c>
       <c r="E63" t="s">
         <v>145</v>
@@ -6719,7 +6895,7 @@
         <v>52</v>
       </c>
       <c r="D64">
-        <v>2.795326114032</v>
+        <v>2.6605802116242914</v>
       </c>
       <c r="E64" t="s">
         <v>145</v>
@@ -6736,7 +6912,7 @@
         <v>53</v>
       </c>
       <c r="D65">
-        <v>2.2633913706480002</v>
+        <v>2.1344238837905145</v>
       </c>
       <c r="E65" t="s">
         <v>145</v>
@@ -6753,7 +6929,7 @@
         <v>54</v>
       </c>
       <c r="D66">
-        <v>1.8486804048160002</v>
+        <v>1.4184653059859922</v>
       </c>
       <c r="E66" t="s">
         <v>145</v>
@@ -6770,7 +6946,7 @@
         <v>55</v>
       </c>
       <c r="D67">
-        <v>1.2956684382880002</v>
+        <v>0.57336241913645269</v>
       </c>
       <c r="E67" t="s">
         <v>145</v>
@@ -6787,7 +6963,7 @@
         <v>56</v>
       </c>
       <c r="D68">
-        <v>0.53186179455679994</v>
+        <v>8.9903298062618056E-2</v>
       </c>
       <c r="E68" t="s">
         <v>145</v>
@@ -6804,7 +6980,7 @@
         <v>57</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>2.9137622653494467E-3</v>
       </c>
       <c r="E69" t="s">
         <v>145</v>
@@ -7025,7 +7201,7 @@
         <v>172</v>
       </c>
       <c r="D82">
-        <v>3.4015238599049997E-3</v>
+        <v>0.15447689350249896</v>
       </c>
       <c r="E82" t="s">
         <v>145</v>
@@ -7042,7 +7218,7 @@
         <v>173</v>
       </c>
       <c r="D83">
-        <v>0.31392081523400001</v>
+        <v>0.98771159810329334</v>
       </c>
       <c r="E83" t="s">
         <v>145</v>
@@ -7059,7 +7235,7 @@
         <v>48</v>
       </c>
       <c r="D84">
-        <v>0.77291755335000001</v>
+        <v>1.9578785595283872</v>
       </c>
       <c r="E84" t="s">
         <v>145</v>
@@ -7076,7 +7252,7 @@
         <v>49</v>
       </c>
       <c r="D85">
-        <v>1.2318703044899999</v>
+        <v>2.5197013456362933</v>
       </c>
       <c r="E85" t="s">
         <v>145</v>
@@ -7093,7 +7269,7 @@
         <v>50</v>
       </c>
       <c r="D86">
-        <v>1.502560154035</v>
+        <v>2.742158349352811</v>
       </c>
       <c r="E86" t="s">
         <v>145</v>
@@ -7110,7 +7286,7 @@
         <v>51</v>
       </c>
       <c r="D87">
-        <v>1.7654465607399998</v>
+        <v>2.71040799692426</v>
       </c>
       <c r="E87" t="s">
         <v>145</v>
@@ -7127,7 +7303,7 @@
         <v>52</v>
       </c>
       <c r="D88">
-        <v>1.848027538175</v>
+        <v>2.5016416250160196</v>
       </c>
       <c r="E88" t="s">
         <v>145</v>
@@ -7144,7 +7320,7 @@
         <v>53</v>
       </c>
       <c r="D89">
-        <v>1.6887293727699997</v>
+        <v>1.9596483403819043</v>
       </c>
       <c r="E89" t="s">
         <v>145</v>
@@ -7161,7 +7337,7 @@
         <v>54</v>
       </c>
       <c r="D90">
-        <v>1.388453274895</v>
+        <v>1.1472564910931693</v>
       </c>
       <c r="E90" t="s">
         <v>145</v>
@@ -7178,7 +7354,7 @@
         <v>55</v>
       </c>
       <c r="D91">
-        <v>0.97934418248499999</v>
+        <v>0.31937275406894788</v>
       </c>
       <c r="E91" t="s">
         <v>145</v>
@@ -7195,7 +7371,7 @@
         <v>56</v>
       </c>
       <c r="D92">
-        <v>0.50532871995999995</v>
+        <v>1.0062283737024223E-2</v>
       </c>
       <c r="E92" t="s">
         <v>145</v>
@@ -7433,7 +7609,7 @@
         <v>172</v>
       </c>
       <c r="D106">
-        <v>9.0707302930800003E-4</v>
+        <v>2.5746148917083163E-2</v>
       </c>
       <c r="E106" t="s">
         <v>145</v>
@@ -7450,7 +7626,7 @@
         <v>173</v>
       </c>
       <c r="D107">
-        <v>8.371221739573334E-2</v>
+        <v>0.16461859968388226</v>
       </c>
       <c r="E107" t="s">
         <v>145</v>
@@ -7467,7 +7643,7 @@
         <v>48</v>
       </c>
       <c r="D108">
-        <v>0.20611134755999999</v>
+        <v>0.32631309325473123</v>
       </c>
       <c r="E108" t="s">
         <v>145</v>
@@ -7484,7 +7660,7 @@
         <v>49</v>
       </c>
       <c r="D109">
-        <v>0.32849874786399996</v>
+        <v>0.41995022427271556</v>
       </c>
       <c r="E109" t="s">
         <v>145</v>
@@ -7501,7 +7677,7 @@
         <v>50</v>
       </c>
       <c r="D110">
-        <v>0.40068270774266662</v>
+        <v>0.45702639155880187</v>
       </c>
       <c r="E110" t="s">
         <v>145</v>
@@ -7518,7 +7694,7 @@
         <v>51</v>
       </c>
       <c r="D111">
-        <v>0.47078574953066671</v>
+        <v>0.4517346661540434</v>
       </c>
       <c r="E111" t="s">
         <v>145</v>
@@ -7535,7 +7711,7 @@
         <v>52</v>
       </c>
       <c r="D112">
-        <v>0.49280734351333333</v>
+        <v>0.41694027083600327</v>
       </c>
       <c r="E112" t="s">
         <v>145</v>
@@ -7552,7 +7728,7 @@
         <v>53</v>
       </c>
       <c r="D113">
-        <v>0.45032783273866656</v>
+        <v>0.3266080567303174</v>
       </c>
       <c r="E113" t="s">
         <v>145</v>
@@ -7569,7 +7745,7 @@
         <v>54</v>
       </c>
       <c r="D114">
-        <v>0.37025420663866665</v>
+        <v>0.19120941518219492</v>
       </c>
       <c r="E114" t="s">
         <v>145</v>
@@ -7586,7 +7762,7 @@
         <v>55</v>
       </c>
       <c r="D115">
-        <v>0.26115844866266669</v>
+        <v>5.3228792344824652E-2</v>
       </c>
       <c r="E115" t="s">
         <v>145</v>
@@ -7603,7 +7779,7 @@
         <v>56</v>
       </c>
       <c r="D116">
-        <v>0.13475432532266665</v>
+        <v>1.6770472895040374E-3</v>
       </c>
       <c r="E116" t="s">
         <v>145</v>
@@ -7824,7 +8000,7 @@
         <v>171</v>
       </c>
       <c r="D129">
-        <v>0</v>
+        <v>6.2472995336241899E-2</v>
       </c>
       <c r="E129" t="s">
         <v>145</v>
@@ -7841,7 +8017,7 @@
         <v>172</v>
       </c>
       <c r="D130">
-        <v>3.4015238599049997E-3</v>
+        <v>0.33472734566972567</v>
       </c>
       <c r="E130" t="s">
         <v>145</v>
@@ -7858,7 +8034,7 @@
         <v>173</v>
       </c>
       <c r="D131">
-        <v>0.31392081523400001</v>
+        <v>0.72055423499322968</v>
       </c>
       <c r="E131" t="s">
         <v>145</v>
@@ -7875,7 +8051,7 @@
         <v>48</v>
       </c>
       <c r="D132">
-        <v>0.77291755335000001</v>
+        <v>1.0599196964378246</v>
       </c>
       <c r="E132" t="s">
         <v>145</v>
@@ -7892,7 +8068,7 @@
         <v>49</v>
       </c>
       <c r="D133">
-        <v>1.2318703044899997</v>
+        <v>1.320780067866874</v>
       </c>
       <c r="E133" t="s">
         <v>145</v>
@@ -7909,7 +8085,7 @@
         <v>50</v>
       </c>
       <c r="D134">
-        <v>1.502560154035</v>
+        <v>1.4694047105628272</v>
       </c>
       <c r="E134" t="s">
         <v>145</v>
@@ -7926,7 +8102,7 @@
         <v>51</v>
       </c>
       <c r="D135">
-        <v>1.7654465607400003</v>
+        <v>1.5161611420356715</v>
       </c>
       <c r="E135" t="s">
         <v>145</v>
@@ -7943,7 +8119,7 @@
         <v>52</v>
       </c>
       <c r="D136">
-        <v>1.848027538175</v>
+        <v>1.4840275479330696</v>
       </c>
       <c r="E136" t="s">
         <v>145</v>
@@ -7960,7 +8136,7 @@
         <v>53</v>
       </c>
       <c r="D137">
-        <v>1.6887293727699997</v>
+        <v>1.4305605870651752</v>
       </c>
       <c r="E137" t="s">
         <v>145</v>
@@ -7977,7 +8153,7 @@
         <v>54</v>
       </c>
       <c r="D138">
-        <v>1.3884532748949998</v>
+        <v>1.2999305283920899</v>
       </c>
       <c r="E138" t="s">
         <v>145</v>
@@ -7994,7 +8170,7 @@
         <v>55</v>
       </c>
       <c r="D139">
-        <v>0.97934418248500021</v>
+        <v>1.0493461043411392</v>
       </c>
       <c r="E139" t="s">
         <v>145</v>
@@ -8011,7 +8187,7 @@
         <v>56</v>
       </c>
       <c r="D140">
-        <v>0.50532871995999984</v>
+        <v>0.73506771643013546</v>
       </c>
       <c r="E140" t="s">
         <v>145</v>
@@ -8028,7 +8204,7 @@
         <v>57</v>
       </c>
       <c r="D141">
-        <v>0</v>
+        <v>0.36772635942697635</v>
       </c>
       <c r="E141" t="s">
         <v>145</v>
@@ -8045,7 +8221,7 @@
         <v>58</v>
       </c>
       <c r="D142">
-        <v>0</v>
+        <v>8.5702020961837433E-2</v>
       </c>
       <c r="E142" t="s">
         <v>145</v>
@@ -8062,7 +8238,7 @@
         <v>59</v>
       </c>
       <c r="D143">
-        <v>0</v>
+        <v>1.6812931481202881E-3</v>
       </c>
       <c r="E143" t="s">
         <v>145</v>
@@ -10911,7 +11087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -11880,8 +12056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11923,7 +12099,7 @@
         <v>2018</v>
       </c>
       <c r="B3" s="15">
-        <v>343.8</v>
+        <v>316.3</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>84</v>
@@ -12040,7 +12216,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A28912B5-8590-412C-8145-960D60FAEF13}">
   <dimension ref="A1:C149"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M69" sqref="M69"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
update on limit, buildyear and bio/nuke fuel price
</commit_message>
<xml_diff>
--- a/projects/virginia/data/data_virginia.xlsx
+++ b/projects/virginia/data/data_virginia.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5072C6-5100-B94E-B8C0-014BAABF2B9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7CF60A-BB55-9642-B537-01C3D6FEBA7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="20500" tabRatio="941" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51200" yWindow="500" windowWidth="25600" windowHeight="21100" tabRatio="941" firstSheet="8" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2307" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2307" uniqueCount="241">
   <si>
     <t>connection</t>
   </si>
@@ -754,10 +754,13 @@
     <t>Ref_MinCapacity</t>
   </si>
   <si>
-    <t>EX_NG_GT_ST</t>
-  </si>
-  <si>
     <t>EX_OIL</t>
+  </si>
+  <si>
+    <t>EX_NG_CT</t>
+  </si>
+  <si>
+    <t>Dominion GT + ST</t>
   </si>
 </sst>
 </file>
@@ -876,7 +879,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -914,6 +917,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1476,8 +1480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1608,8 +1612,8 @@
       <c r="A3" t="s">
         <v>114</v>
       </c>
-      <c r="B3">
-        <v>5</v>
+      <c r="B3" s="25">
+        <v>2.86</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1740,8 +1744,11 @@
       <c r="A10" t="s">
         <v>185</v>
       </c>
-      <c r="B10">
-        <v>1.94</v>
+      <c r="B10" s="25">
+        <v>0.6</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
       </c>
       <c r="J10">
         <v>50</v>
@@ -1807,7 +1814,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1909,7 +1916,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>174</v>
@@ -1987,7 +1994,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>175</v>
@@ -2491,7 +2498,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2582,7 +2589,7 @@
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="5">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>183</v>
@@ -2590,7 +2597,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B4" s="32">
         <v>85</v>
@@ -2607,7 +2614,7 @@
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="6">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>183</v>
@@ -2657,7 +2664,7 @@
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="5">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>183</v>
@@ -2665,7 +2672,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B7" s="33">
         <v>30</v>
@@ -2682,7 +2689,7 @@
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="5">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>183</v>
@@ -3124,7 +3131,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3174,10 +3181,10 @@
       <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="L1" s="3" t="s">
         <v>225</v>
       </c>
     </row>
@@ -3212,10 +3219,10 @@
       <c r="J2" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="L2" s="2" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3245,7 +3252,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -3317,7 +3324,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -3845,7 +3852,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3939,7 +3946,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B4" s="5">
         <v>0.67</v>
@@ -3971,7 +3978,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -4057,7 +4064,9 @@
       </c>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
-      <c r="D14" s="18"/>
+      <c r="D14" s="37">
+        <v>300</v>
+      </c>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
@@ -4073,7 +4082,7 @@
         <v>0.01</v>
       </c>
       <c r="C15" s="18"/>
-      <c r="D15" s="18">
+      <c r="D15" s="25">
         <v>8000</v>
       </c>
       <c r="E15" s="18"/>
@@ -4087,7 +4096,9 @@
       <c r="A16" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="18"/>
+      <c r="B16" s="18">
+        <v>0.01</v>
+      </c>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
@@ -4147,8 +4158,8 @@
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
-      <c r="D20" s="18">
-        <v>20000</v>
+      <c r="D20" s="25">
+        <v>40000</v>
       </c>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
@@ -4161,7 +4172,7 @@
       <c r="A21" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="25">
         <v>5200</v>
       </c>
       <c r="H21" s="31">
@@ -4203,8 +4214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4250,7 +4261,7 @@
         <v>3780</v>
       </c>
       <c r="C3">
-        <v>1985</v>
+        <v>1964</v>
       </c>
       <c r="D3" t="s">
         <v>199</v>
@@ -4258,13 +4269,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B4">
         <v>2343</v>
       </c>
       <c r="C4">
-        <v>1980</v>
+        <v>1967</v>
       </c>
       <c r="D4" t="s">
         <v>200</v>
@@ -4278,7 +4289,7 @@
         <v>866</v>
       </c>
       <c r="C5">
-        <v>2010</v>
+        <v>1985</v>
       </c>
       <c r="D5" t="s">
         <v>195</v>
@@ -4292,7 +4303,7 @@
         <v>4695</v>
       </c>
       <c r="C6">
-        <v>1995</v>
+        <v>1990</v>
       </c>
       <c r="D6" t="s">
         <v>198</v>
@@ -4314,16 +4325,16 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B8">
         <v>5317</v>
       </c>
       <c r="C8">
-        <v>1995</v>
+        <v>1990</v>
       </c>
       <c r="D8" t="s">
-        <v>198</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4376,7 +4387,7 @@
         <v>892</v>
       </c>
       <c r="C12">
-        <v>2013</v>
+        <v>1992</v>
       </c>
       <c r="D12" t="s">
         <v>194</v>
@@ -4390,7 +4401,7 @@
         <v>3241</v>
       </c>
       <c r="C13">
-        <v>1970</v>
+        <v>1985</v>
       </c>
       <c r="D13" t="s">
         <v>204</v>
@@ -9978,7 +9989,7 @@
   <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10829,7 +10840,7 @@
         <v>2018</v>
       </c>
       <c r="B3" s="15">
-        <v>302.8</v>
+        <v>310.5</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
reserve margin/oil/fuel price update
</commit_message>
<xml_diff>
--- a/projects/virginia/data/data_virginia.xlsx
+++ b/projects/virginia/data/data_virginia.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309D46DA-4409-F74B-B8E1-ADA7F991E460}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CF9CCE-CB51-AB41-B9DD-B473C2DE5B1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="21100" tabRatio="941" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25600" yWindow="500" windowWidth="25600" windowHeight="21100" tabRatio="941" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -829,9 +829,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000000000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -900,8 +900,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -943,6 +957,16 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -953,13 +977,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -981,7 +1007,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -997,11 +1023,16 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="5" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="5" builtinId="29"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -1561,8 +1592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1710,7 +1741,7 @@
       <c r="B3" s="35">
         <v>2.86</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="37">
         <v>2</v>
       </c>
       <c r="D3" s="10" t="s">
@@ -1738,8 +1769,8 @@
       <c r="A4" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="35">
-        <v>1.95</v>
+      <c r="B4" s="38">
+        <v>2.75</v>
       </c>
       <c r="C4" s="35">
         <v>-0.1</v>
@@ -1778,8 +1809,8 @@
       <c r="A6" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="35">
-        <v>14.6</v>
+      <c r="B6" s="38">
+        <v>11.29</v>
       </c>
       <c r="C6" s="35">
         <v>3.6</v>
@@ -1804,8 +1835,8 @@
       <c r="A7" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="35">
-        <v>2.79</v>
+      <c r="B7" s="38">
+        <v>3.91</v>
       </c>
       <c r="C7" s="35">
         <v>1.1000000000000001</v>
@@ -1949,7 +1980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -3408,7 +3439,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3534,8 +3565,8 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="E4" s="32">
-        <v>13</v>
+      <c r="E4" s="39">
+        <v>12.9</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -3889,7 +3920,7 @@
         <v>244</v>
       </c>
       <c r="E17">
-        <v>13</v>
+        <v>12.9</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -4944,7 +4975,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4970,9 +5001,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>0.36399999999999999</v>
+    <row r="3" spans="1:2" ht="16">
+      <c r="A3" s="38">
+        <v>0.41860000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -4984,7 +5015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E290"/>
   <sheetViews>
-    <sheetView topLeftCell="A211" workbookViewId="0">
+    <sheetView topLeftCell="A205" workbookViewId="0">
       <selection activeCell="I232" sqref="I232"/>
     </sheetView>
   </sheetViews>

</xml_diff>